<commit_message>
some updates to slides for more intuition
</commit_message>
<xml_diff>
--- a/materials/capital-investment-decisions.xlsx
+++ b/materials/capital-investment-decisions.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/quinference/Documents/Corporate-Finance-Management/corp-fin-mgt/materials/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{244EBE8B-3514-BD46-9E9F-FFFBE5D88A79}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{916CA4A4-F7ED-C14B-B073-F5E3B9522464}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="160" yWindow="920" windowWidth="17040" windowHeight="10540" firstSheet="5" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="160" yWindow="920" windowWidth="17040" windowHeight="21260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="1_Dashboard" sheetId="1" r:id="rId1"/>
@@ -20,13 +20,9 @@
     <sheet name="5_IRR" sheetId="5" r:id="rId5"/>
     <sheet name="6_ARR" sheetId="6" r:id="rId6"/>
     <sheet name="7_Method_Comparison" sheetId="7" r:id="rId7"/>
-    <sheet name="8_Risk_Analysis" sheetId="8" r:id="rId8"/>
-    <sheet name="9_Case_Study" sheetId="9" r:id="rId9"/>
-    <sheet name="8_Risk_Analysis_Updated" sheetId="10" r:id="rId10"/>
+    <sheet name="8_Risk_Analysis_Updated" sheetId="10" r:id="rId8"/>
+    <sheet name="9_Case_Study " sheetId="11" r:id="rId9"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId11"/>
-  </externalReferences>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -45,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="143">
   <si>
     <t>Discounted Payback Period (DPP)</t>
   </si>
@@ -341,30 +337,12 @@
     <t>Expected Value</t>
   </si>
   <si>
-    <t>Expected NPV Calculation:</t>
-  </si>
-  <si>
-    <t>Risk-Adjusted Discount Rate:</t>
-  </si>
-  <si>
-    <t>Chart: Risk-Return Relationship</t>
-  </si>
-  <si>
     <t>Case Study: Evaluating a New Plumbing Business Venture</t>
   </si>
   <si>
-    <t>This worksheet provides a complete analysis of the plumbing business case from the lecture slides.</t>
-  </si>
-  <si>
-    <t>Business Plan Overview:</t>
-  </si>
-  <si>
     <t>Notes</t>
   </si>
   <si>
-    <t>Initial investment (Equipment: £25,000, Van: £15,000, Advertising: £5,000)</t>
-  </si>
-  <si>
     <t>Year 1 operations</t>
   </si>
   <si>
@@ -377,9 +355,6 @@
     <t>Year 4 operations</t>
   </si>
   <si>
-    <t>Year 5 operations + Exit value (Business: £30,000, Equipment: £8,000, Van: £3,000)</t>
-  </si>
-  <si>
     <t>Comprehensive Appraisal:</t>
   </si>
   <si>
@@ -443,30 +418,6 @@
     <t>- Click worksheet tabs at the bottom to navigate between topics</t>
   </si>
   <si>
-    <t>Project Dashboard - Current Selection: Plumbing Business Case</t>
-  </si>
-  <si>
-    <t>Key Metrics Summary (linked values from other sheets):</t>
-  </si>
-  <si>
-    <t>Payback Period:</t>
-  </si>
-  <si>
-    <t>Discounted Payback Period:</t>
-  </si>
-  <si>
-    <t>NPV:</t>
-  </si>
-  <si>
-    <t>IRR:</t>
-  </si>
-  <si>
-    <t>Residual Value (£)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> </t>
-  </si>
-  <si>
     <t>Discount Rate Sensitivity Table:</t>
   </si>
   <si>
@@ -477,24 +428,55 @@
   </si>
   <si>
     <t>IRR (%)</t>
+  </si>
+  <si>
+    <t>This worksheet provides a complete financial appraisal, risk analysis, and decision support for the plumbing business case.</t>
+  </si>
+  <si>
+    <t>Initial investment</t>
+  </si>
+  <si>
+    <t>Year 5 operations + Exit value</t>
+  </si>
+  <si>
+    <t>Accounting Rate of Return (ARR):</t>
+  </si>
+  <si>
+    <t>Payback Period (approx):</t>
+  </si>
+  <si>
+    <t>Discounted Payback Period (approx):</t>
+  </si>
+  <si>
+    <t>Sensitivity to Initial Investment (break-even level):</t>
+  </si>
+  <si>
+    <t>Sensitivity to Residual Value (to offset shortfall):</t>
+  </si>
+  <si>
+    <t>Break-even Discount Rate:</t>
+  </si>
+  <si>
+    <t>Final Recommendation:</t>
+  </si>
+  <si>
+    <t>Change Initial Investment (£):</t>
+  </si>
+  <si>
+    <t>Change Discount Rate:</t>
+  </si>
+  <si>
+    <t>Updated NPV:</t>
+  </si>
+  <si>
+    <t>Updated IRR:</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
-    <numFmt numFmtId="6" formatCode="&quot;£&quot;#,##0_);[Red]\(&quot;£&quot;#,##0\)"/>
-    <numFmt numFmtId="171" formatCode="&quot;£&quot;#,##0"/>
-  </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -532,23 +514,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="171" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="6" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="6" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="9" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="9" fontId="0" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Per cent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -1028,87 +1003,6 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <xxl21:alternateUrls>
-      <xxl21:absoluteUrl r:id="rId2"/>
-    </xxl21:alternateUrls>
-    <sheetNames>
-      <sheetName val="8_Risk_Analysis_Updated"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0">
-        <row r="52">
-          <cell r="A52">
-            <v>0.05</v>
-          </cell>
-          <cell r="B52">
-            <v>155966.88230775867</v>
-          </cell>
-        </row>
-        <row r="53">
-          <cell r="A53">
-            <v>7.4999999999999997E-2</v>
-          </cell>
-          <cell r="B53">
-            <v>115798.79463113565</v>
-          </cell>
-        </row>
-        <row r="54">
-          <cell r="A54">
-            <v>0.1</v>
-          </cell>
-          <cell r="B54">
-            <v>79440.674072188209</v>
-          </cell>
-        </row>
-        <row r="55">
-          <cell r="A55">
-            <v>0.125</v>
-          </cell>
-          <cell r="B55">
-            <v>46430.25284086098</v>
-          </cell>
-        </row>
-        <row r="56">
-          <cell r="A56">
-            <v>0.15</v>
-          </cell>
-          <cell r="B56">
-            <v>16371.95220950793</v>
-          </cell>
-        </row>
-        <row r="62">
-          <cell r="B62">
-            <v>40000</v>
-          </cell>
-          <cell r="C62">
-            <v>0.08</v>
-          </cell>
-        </row>
-        <row r="63">
-          <cell r="B63">
-            <v>80000</v>
-          </cell>
-          <cell r="C63">
-            <v>0.12</v>
-          </cell>
-        </row>
-        <row r="64">
-          <cell r="B64">
-            <v>120000</v>
-          </cell>
-          <cell r="C64">
-            <v>0.16</v>
-          </cell>
-        </row>
-      </sheetData>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -1394,521 +1288,101 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C31"/>
+  <dimension ref="A1:A21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A23" sqref="A23:D31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>116</v>
+        <v>109</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>118</v>
+        <v>111</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>120</v>
+        <v>113</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>122</v>
+        <v>115</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>123</v>
+        <v>116</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B23" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B25" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B27" t="s">
-        <v>134</v>
-      </c>
-      <c r="C27" t="e">
-        <v>#REF!</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B28" t="s">
-        <v>135</v>
-      </c>
-      <c r="C28" t="e">
-        <v>#REF!</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B29" t="s">
-        <v>136</v>
-      </c>
-      <c r="C29" t="e">
-        <v>#REF!</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B30" t="s">
-        <v>137</v>
-      </c>
-      <c r="C30" t="e">
-        <v>#REF!</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B31" t="s">
-        <v>57</v>
-      </c>
-      <c r="C31" t="e">
-        <v>#REF!</v>
+        <v>124</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{888E53AA-FD86-EB41-A67D-20D7AA9B1FC1}">
-  <dimension ref="A1:F64"/>
-  <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
-      <selection activeCell="J23" sqref="J23"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>3</v>
-      </c>
-      <c r="B7" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A8">
-        <v>0</v>
-      </c>
-      <c r="B8" s="1">
-        <v>-500000</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A9">
-        <v>1</v>
-      </c>
-      <c r="B9" s="1">
-        <v>150000</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A10">
-        <v>2</v>
-      </c>
-      <c r="B10" s="1">
-        <v>180000</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A11">
-        <v>3</v>
-      </c>
-      <c r="B11" s="1">
-        <v>200000</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A12">
-        <v>4</v>
-      </c>
-      <c r="B12" s="1">
-        <v>120000</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A13">
-        <v>5</v>
-      </c>
-      <c r="B13" s="1">
-        <v>100000</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
-        <v>83</v>
-      </c>
-      <c r="B17" t="s">
-        <v>84</v>
-      </c>
-      <c r="C17" t="s">
-        <v>85</v>
-      </c>
-      <c r="D17" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A18" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="B18" s="1">
-        <f>ABS(B8)</f>
-        <v>500000</v>
-      </c>
-      <c r="C18" s="2">
-        <f>ROUND(NPV(D21,B9:B13),0)</f>
-        <v>750000</v>
-      </c>
-      <c r="D18" s="2">
-        <f>(C18-B18)/B18</f>
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A19" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="C19" s="2"/>
-      <c r="D19" s="2"/>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A20" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="B20" s="1">
-        <v>0</v>
-      </c>
-      <c r="C20" s="2">
-        <f>-(NPV(D21,B9:B13)+B8)*(1+D21)^5</f>
-        <v>-250000</v>
-      </c>
-      <c r="D20" s="2" t="str">
-        <f>IF(B20&lt;&gt;0,(C20-B20)/B20,"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A21" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="B21" s="1">
-        <v>0.1</v>
-      </c>
-      <c r="C21" s="2">
-        <f>IRR(B8:B13)</f>
-        <v>0.16464215163431573</v>
-      </c>
-      <c r="D21" s="2"/>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A30" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A32" t="s">
-        <v>90</v>
-      </c>
-      <c r="B32" t="s">
-        <v>91</v>
-      </c>
-      <c r="C32" t="s">
-        <v>92</v>
-      </c>
-      <c r="D32" t="s">
-        <v>93</v>
-      </c>
-      <c r="E32" t="s">
-        <v>38</v>
-      </c>
-      <c r="F32" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A33" t="s">
-        <v>94</v>
-      </c>
-      <c r="B33" s="1">
-        <v>0.25</v>
-      </c>
-      <c r="C33" s="1">
-        <v>0.05</v>
-      </c>
-      <c r="D33" s="1">
-        <v>1</v>
-      </c>
-      <c r="E33" s="1">
-        <v>40000</v>
-      </c>
-      <c r="F33" s="1">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A34" t="s">
-        <v>95</v>
-      </c>
-      <c r="B34" s="1">
-        <v>0.5</v>
-      </c>
-      <c r="C34" s="1">
-        <v>0.1</v>
-      </c>
-      <c r="D34" s="1">
-        <v>1.5</v>
-      </c>
-      <c r="E34" s="1">
-        <v>80000</v>
-      </c>
-      <c r="F34" s="1">
-        <v>0.12</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A35" t="s">
-        <v>96</v>
-      </c>
-      <c r="B35" s="1">
-        <v>0.25</v>
-      </c>
-      <c r="C35" s="1">
-        <v>0.15</v>
-      </c>
-      <c r="D35" s="1">
-        <v>2</v>
-      </c>
-      <c r="E35" s="1">
-        <v>120000</v>
-      </c>
-      <c r="F35" s="1">
-        <v>0.16</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A36" t="s">
-        <v>97</v>
-      </c>
-      <c r="B36" s="1">
-        <v>1</v>
-      </c>
-      <c r="E36" s="2">
-        <f>SUMPRODUCT(B31:B33,E31:E33)</f>
-        <v>10000</v>
-      </c>
-      <c r="F36" s="2">
-        <f>SUMPRODUCT(B31:B33,F31:F33)</f>
-        <v>0.02</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A50" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A51" t="s">
-        <v>37</v>
-      </c>
-      <c r="B51" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A52" s="1">
-        <v>0.05</v>
-      </c>
-      <c r="B52" s="2">
-        <f>NPV(A52,B9:B13)+B8</f>
-        <v>155966.88230775867</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A53" s="1">
-        <v>7.4999999999999997E-2</v>
-      </c>
-      <c r="B53" s="2">
-        <f>NPV(A53,B9:B13)+B8</f>
-        <v>115798.79463113565</v>
-      </c>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A54" s="1">
-        <v>0.1</v>
-      </c>
-      <c r="B54" s="2">
-        <f>NPV(A54,B9:B13)+B8</f>
-        <v>79440.674072188209</v>
-      </c>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A55" s="1">
-        <v>0.125</v>
-      </c>
-      <c r="B55" s="2">
-        <f>NPV(A55,B9:B13)+B8</f>
-        <v>46430.25284086098</v>
-      </c>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A56" s="1">
-        <v>0.15</v>
-      </c>
-      <c r="B56" s="2">
-        <f>NPV(A56,B9:B13)+B8</f>
-        <v>16371.95220950793</v>
-      </c>
-    </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A60" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A61" t="s">
-        <v>90</v>
-      </c>
-      <c r="B61" t="s">
-        <v>141</v>
-      </c>
-      <c r="C61" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A62" t="s">
-        <v>94</v>
-      </c>
-      <c r="B62" s="1">
-        <v>40000</v>
-      </c>
-      <c r="C62" s="1">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A63" t="s">
-        <v>95</v>
-      </c>
-      <c r="B63" s="1">
-        <v>80000</v>
-      </c>
-      <c r="C63" s="1">
-        <v>0.12</v>
-      </c>
-    </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A64" t="s">
-        <v>96</v>
-      </c>
-      <c r="B64" s="1">
-        <v>120000</v>
-      </c>
-      <c r="C64" s="1">
-        <v>0.16</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -3458,28 +2932,396 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
-  <dimension ref="A1:G50"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{888E53AA-FD86-EB41-A67D-20D7AA9B1FC1}">
+  <dimension ref="A1:F64"/>
   <sheetViews>
     <sheetView topLeftCell="A42" workbookViewId="0">
-      <selection activeCell="A35" sqref="A35"/>
+      <selection activeCell="J23" sqref="J23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>3</v>
+      </c>
+      <c r="B7" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>0</v>
+      </c>
+      <c r="B8" s="1">
+        <v>-500000</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>1</v>
+      </c>
+      <c r="B9" s="1">
+        <v>150000</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>2</v>
+      </c>
+      <c r="B10" s="1">
+        <v>180000</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>3</v>
+      </c>
+      <c r="B11" s="1">
+        <v>200000</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>4</v>
+      </c>
+      <c r="B12" s="1">
+        <v>120000</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>5</v>
+      </c>
+      <c r="B13" s="1">
+        <v>100000</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>83</v>
+      </c>
+      <c r="B17" t="s">
+        <v>84</v>
+      </c>
+      <c r="C17" t="s">
+        <v>85</v>
+      </c>
+      <c r="D17" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A18" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B18" s="1">
+        <f>ABS(B8)</f>
+        <v>500000</v>
+      </c>
+      <c r="C18" s="2">
+        <f>ROUND(NPV(D21,B9:B13),0)</f>
+        <v>750000</v>
+      </c>
+      <c r="D18" s="2">
+        <f>(C18-B18)/B18</f>
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A19" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="C19" s="2"/>
+      <c r="D19" s="2"/>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A20" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B20" s="1">
+        <v>0</v>
+      </c>
+      <c r="C20" s="2">
+        <f>-(NPV(D21,B9:B13)+B8)*(1+D21)^5</f>
+        <v>-250000</v>
+      </c>
+      <c r="D20" s="2" t="str">
+        <f>IF(B20&lt;&gt;0,(C20-B20)/B20,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A21" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B21" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="C21" s="2">
+        <f>IRR(B8:B13)</f>
+        <v>0.16464215163431573</v>
+      </c>
+      <c r="D21" s="2"/>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>90</v>
+      </c>
+      <c r="B32" t="s">
+        <v>91</v>
+      </c>
+      <c r="C32" t="s">
+        <v>92</v>
+      </c>
+      <c r="D32" t="s">
+        <v>93</v>
+      </c>
+      <c r="E32" t="s">
+        <v>38</v>
+      </c>
+      <c r="F32" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>94</v>
+      </c>
+      <c r="B33" s="1">
+        <v>0.25</v>
+      </c>
+      <c r="C33" s="1">
+        <v>0.05</v>
+      </c>
+      <c r="D33" s="1">
+        <v>1</v>
+      </c>
+      <c r="E33" s="1">
+        <v>40000</v>
+      </c>
+      <c r="F33" s="1">
+        <v>0.08</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>95</v>
+      </c>
+      <c r="B34" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="C34" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="D34" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="E34" s="1">
+        <v>80000</v>
+      </c>
+      <c r="F34" s="1">
+        <v>0.12</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>96</v>
+      </c>
+      <c r="B35" s="1">
+        <v>0.25</v>
+      </c>
+      <c r="C35" s="1">
+        <v>0.15</v>
+      </c>
+      <c r="D35" s="1">
+        <v>2</v>
+      </c>
+      <c r="E35" s="1">
+        <v>120000</v>
+      </c>
+      <c r="F35" s="1">
+        <v>0.16</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>97</v>
+      </c>
+      <c r="B36" s="1">
+        <v>1</v>
+      </c>
+      <c r="E36" s="2">
+        <f>SUMPRODUCT(B31:B33,E31:E33)</f>
+        <v>10000</v>
+      </c>
+      <c r="F36" s="2">
+        <f>SUMPRODUCT(B31:B33,F31:F33)</f>
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
+        <v>37</v>
+      </c>
+      <c r="B51" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A52" s="1">
+        <v>0.05</v>
+      </c>
+      <c r="B52" s="2">
+        <f>NPV(A52,B9:B13)+B8</f>
+        <v>155966.88230775867</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A53" s="1">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="B53" s="2">
+        <f>NPV(A53,B9:B13)+B8</f>
+        <v>115798.79463113565</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A54" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="B54" s="2">
+        <f>NPV(A54,B9:B13)+B8</f>
+        <v>79440.674072188209</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A55" s="1">
+        <v>0.125</v>
+      </c>
+      <c r="B55" s="2">
+        <f>NPV(A55,B9:B13)+B8</f>
+        <v>46430.25284086098</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A56" s="1">
+        <v>0.15</v>
+      </c>
+      <c r="B56" s="2">
+        <f>NPV(A56,B9:B13)+B8</f>
+        <v>16371.95220950793</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A60" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A61" t="s">
+        <v>90</v>
+      </c>
+      <c r="B61" t="s">
+        <v>126</v>
+      </c>
+      <c r="C61" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A62" t="s">
+        <v>94</v>
+      </c>
+      <c r="B62" s="1">
+        <v>40000</v>
+      </c>
+      <c r="C62" s="1">
+        <v>0.08</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A63" t="s">
+        <v>95</v>
+      </c>
+      <c r="B63" s="1">
+        <v>80000</v>
+      </c>
+      <c r="C63" s="1">
+        <v>0.12</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A64" t="s">
+        <v>96</v>
+      </c>
+      <c r="B64" s="1">
+        <v>120000</v>
+      </c>
+      <c r="C64" s="1">
+        <v>0.16</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{467627C5-3AB8-7747-A40F-4D04993626A5}">
+  <dimension ref="A1:G37"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A43" sqref="A43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="84.5" customWidth="1"/>
-    <col min="2" max="2" width="13.6640625" customWidth="1"/>
-    <col min="3" max="3" width="16.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="94.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>80</v>
+        <v>98</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>81</v>
+        <v>129</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
@@ -3494,367 +3336,215 @@
       <c r="B7" t="s">
         <v>4</v>
       </c>
-      <c r="G7" t="s">
-        <v>139</v>
+      <c r="C7" t="s">
+        <v>99</v>
+      </c>
+      <c r="F7" t="s">
+        <v>63</v>
+      </c>
+      <c r="G7" s="1">
+        <v>0.1</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>0</v>
       </c>
-      <c r="B8" s="3">
-        <v>-500000</v>
-      </c>
-      <c r="G8" t="s">
-        <v>139</v>
+      <c r="B8" s="1">
+        <v>-45000</v>
+      </c>
+      <c r="C8" t="s">
+        <v>130</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>1</v>
       </c>
-      <c r="B9" s="3">
-        <v>150000</v>
-      </c>
-      <c r="G9" t="s">
-        <v>138</v>
+      <c r="B9" s="1">
+        <v>12000</v>
+      </c>
+      <c r="C9" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>2</v>
       </c>
-      <c r="B10" s="3">
-        <v>180000</v>
-      </c>
-      <c r="G10">
-        <v>10000</v>
+      <c r="B10" s="1">
+        <v>18000</v>
+      </c>
+      <c r="C10" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>3</v>
       </c>
-      <c r="B11" s="3">
-        <v>200000</v>
+      <c r="B11" s="1">
+        <v>22000</v>
+      </c>
+      <c r="C11" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>4</v>
       </c>
-      <c r="B12" s="3">
-        <v>120000</v>
+      <c r="B12" s="1">
+        <v>25000</v>
+      </c>
+      <c r="C12" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>5</v>
       </c>
-      <c r="B13" s="3">
-        <v>100000</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B13" s="1">
+        <v>67000</v>
+      </c>
+      <c r="C13" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>83</v>
-      </c>
-      <c r="B17" t="s">
-        <v>84</v>
-      </c>
-      <c r="C17" t="s">
-        <v>85</v>
-      </c>
-      <c r="D17" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A18" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="B18" s="4">
-        <f>ABS(B8)</f>
-        <v>500000</v>
-      </c>
-      <c r="C18" s="5">
-        <f>ROUND(SUM(NPV($VB$21,B8:B12)), 0)</f>
-        <v>150000</v>
-      </c>
-      <c r="D18" s="1">
-        <f>(C18 - B18) / B18</f>
-        <v>-0.7</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A19" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="C19" s="1"/>
-      <c r="D19" s="1"/>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A20" s="1" t="s">
-        <v>50</v>
+        <v>27</v>
+      </c>
+      <c r="B17" s="2">
+        <f>NPV(G7,B9:B13)+B8</f>
+        <v>55991.114615866987</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>33</v>
+      </c>
+      <c r="B18" s="2">
+        <f>IRR(B8:B13)</f>
+        <v>0.39737798465480045</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>132</v>
+      </c>
+      <c r="B19" s="2">
+        <f>AVERAGE(B9:B13)/((ABS(B8)+0)/2)</f>
+        <v>1.28</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>133</v>
       </c>
       <c r="B20" s="2">
-        <f>G10</f>
-        <v>10000</v>
-      </c>
-      <c r="C20" s="1">
-        <f>-(NPV(B21,B9:B13)+B8)*(1+B21)^5</f>
-        <v>-127939.99999999987</v>
-      </c>
-      <c r="D20" s="1">
-        <f>(C20 - B20) / B20</f>
-        <v>-13.793999999999988</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A21" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="B21" s="7">
+        <f>3+ABS(SUM(B8:B11)/B12)</f>
+        <v>3.2800000000000002</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>134</v>
+      </c>
+      <c r="B21" s="2">
+        <f>3+ABS((NPV(G7,B9:B11)+B8)/((B12/(1+G7)^4)))</f>
+        <v>3.1573000000000002</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>135</v>
+      </c>
+      <c r="B25" s="2">
+        <f>ROUND(NPV(G7,B9:B13),0)</f>
+        <v>100991</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>136</v>
+      </c>
+      <c r="B26" s="2">
+        <f>-(NPV(G7,B9:B13)+B8)*(1+G7)^5</f>
+        <v>-90174.249999999971</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>137</v>
+      </c>
+      <c r="B27" s="2">
+        <f>IRR(B8:B13)</f>
+        <v>0.39737798465480045</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>138</v>
+      </c>
+      <c r="B30" s="2" t="str">
+        <f>IF(AND(B17&gt;0, B18&gt;G7, B19&gt;0.15), "ACCEPT", "REJECT")</f>
+        <v>ACCEPT</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>139</v>
+      </c>
+      <c r="B33" s="1">
+        <v>-45000</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>140</v>
+      </c>
+      <c r="B34" s="1">
         <v>0.1</v>
       </c>
-      <c r="C21" s="6">
-        <f>IRR(B8:B13)</f>
-        <v>0.16464215163431573</v>
-      </c>
-      <c r="D21" s="1"/>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A27" t="s">
-        <v>90</v>
-      </c>
-      <c r="B27" t="s">
-        <v>91</v>
-      </c>
-      <c r="C27" t="s">
-        <v>92</v>
-      </c>
-      <c r="D27" t="s">
-        <v>93</v>
-      </c>
-      <c r="E27" t="s">
-        <v>38</v>
-      </c>
-      <c r="F27" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A28" t="s">
-        <v>94</v>
-      </c>
-      <c r="B28" s="1">
-        <v>0.25</v>
-      </c>
-      <c r="C28" s="1">
-        <v>0.05</v>
-      </c>
-      <c r="D28" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A29" t="s">
-        <v>95</v>
-      </c>
-      <c r="B29" s="1">
-        <v>0.5</v>
-      </c>
-      <c r="C29" s="1">
-        <v>0.1</v>
-      </c>
-      <c r="D29" s="1">
-        <v>1.5</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A30" t="s">
-        <v>96</v>
-      </c>
-      <c r="B30" s="1">
-        <v>0.25</v>
-      </c>
-      <c r="C30" s="1">
-        <v>0.15</v>
-      </c>
-      <c r="D30" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A31" t="s">
-        <v>97</v>
-      </c>
-      <c r="B31" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A35" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A40" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A50" t="s">
-        <v>100</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
-  <dimension ref="A1:G50"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
-        <v>3</v>
-      </c>
-      <c r="B18" t="s">
-        <v>4</v>
-      </c>
-      <c r="C18" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A19">
-        <v>0</v>
-      </c>
-      <c r="B19" s="1">
-        <v>-45000</v>
-      </c>
-      <c r="C19" t="s">
-        <v>105</v>
-      </c>
-      <c r="F19" t="s">
-        <v>63</v>
-      </c>
-      <c r="G19" s="1">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A20">
-        <v>1</v>
-      </c>
-      <c r="B20" s="1">
-        <v>12000</v>
-      </c>
-      <c r="C20" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A21">
-        <v>2</v>
-      </c>
-      <c r="B21" s="1">
-        <v>18000</v>
-      </c>
-      <c r="C21" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A22">
-        <v>3</v>
-      </c>
-      <c r="B22" s="1">
-        <v>22000</v>
-      </c>
-      <c r="C22" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A23">
-        <v>4</v>
-      </c>
-      <c r="B23" s="1">
-        <v>25000</v>
-      </c>
-      <c r="C23" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A24">
-        <v>5</v>
-      </c>
-      <c r="B24" s="1">
-        <v>67000</v>
-      </c>
-      <c r="C24" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A27" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A35" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A45" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A50" t="s">
-        <v>114</v>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>141</v>
+      </c>
+      <c r="B36" s="2">
+        <f>NPV(B34,B9:B13)+B33</f>
+        <v>55991.114615866987</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>142</v>
+      </c>
+      <c r="B37" s="2">
+        <f>IRR(B13:B33)</f>
+        <v>-0.1105619331545481</v>
       </c>
     </row>
   </sheetData>

</xml_diff>